<commit_message>
Added Testdata and Thread Local Implementation
</commit_message>
<xml_diff>
--- a/data/caseAndLegalEntity.xlsx
+++ b/data/caseAndLegalEntity.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3A27E8E1-BC81-48EF-8F31-AC8BE7E735DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Our Folder\Maven project\PageObjectModel_SalesForce\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60573606-8A53-4ADA-B927-7CD92F27FB16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="23304" windowHeight="13224" firstSheet="6" activeTab="9" xr2:uid="{8775F28F-7B0A-42D9-998A-F450B9A9F440}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="1" xr2:uid="{8775F28F-7B0A-42D9-998A-F450B9A9F440}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Create_NewCase" sheetId="2" r:id="rId2"/>
     <sheet name="EditCase" sheetId="7" r:id="rId3"/>
     <sheet name="DeleteCase" sheetId="8" r:id="rId4"/>
-    <sheet name="Create_New_LegalEntity" sheetId="5" r:id="rId5"/>
-    <sheet name="Edit_LegalEntity" sheetId="6" r:id="rId6"/>
-    <sheet name="Verify_LegalEntities_SortBy" sheetId="9" r:id="rId7"/>
-    <sheet name="Create_NewOrder" sheetId="10" r:id="rId8"/>
-    <sheet name="Edit_Order" sheetId="11" r:id="rId9"/>
+    <sheet name="Create_NewOrder" sheetId="13" r:id="rId5"/>
+    <sheet name="Edit_Order" sheetId="14" r:id="rId6"/>
+    <sheet name="Create_New_LegalEntity" sheetId="5" r:id="rId7"/>
+    <sheet name="Edit_LegalEntity" sheetId="6" r:id="rId8"/>
+    <sheet name="Verify_LegalEntities_SortBy" sheetId="9" r:id="rId9"/>
     <sheet name="File" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -41,9 +45,6 @@
     <t>cypress@testleaf.com</t>
   </si>
   <si>
-    <t>Bootcamp@123</t>
-  </si>
-  <si>
     <t>ContactName</t>
   </si>
   <si>
@@ -53,9 +54,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>saran</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
@@ -68,9 +66,6 @@
     <t>Saran_3012dak</t>
   </si>
   <si>
-    <t>Salesforce Automation by Saranya</t>
-  </si>
-  <si>
     <t>SearchByName</t>
   </si>
   <si>
@@ -84,6 +79,24 @@
   </si>
   <si>
     <t>Selbootcamp@123</t>
+  </si>
+  <si>
+    <t>Salesforce Automation by SaranyaJegan</t>
+  </si>
+  <si>
+    <t>Saran</t>
+  </si>
+  <si>
+    <t>AccountName</t>
+  </si>
+  <si>
+    <t>ContractNumber</t>
+  </si>
+  <si>
+    <t>0000010</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -107,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +130,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,10 +153,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -456,7 +477,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,13 +499,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{4556AEDF-4EC3-4A1C-9553-4A115ADFA49A}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{D536F2EB-54D6-4931-87D9-1FE8FDACC079}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{EDC4EF7D-F916-4794-A13B-8C47AF8D49B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -494,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF9B971-C059-4945-8FDF-F7ACB83B89D7}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,7 +538,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -533,12 +554,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD93B44-F2C1-46D3-9D76-6E9FF921864E}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" customWidth="1"/>
@@ -552,13 +574,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -566,22 +588,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{FBDEFE17-8BE2-4891-8128-8271EFA20630}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{B1A64133-C4BE-4921-9681-F0072A436882}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{68C5D0E0-F35A-4E45-83E9-42B7B5B52E1C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -592,7 +614,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,13 +636,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{07AE2198-5C92-41FA-BE62-DFEA6A1CB137}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{2ABF30CE-C34E-4E6C-B254-702256F77CBD}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{0683A397-5159-427A-A59F-D5F948E849BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -653,24 +675,119 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{EE89F3B7-7A76-42C1-8560-09941F5B894A}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{A8AF62F0-DC05-4562-AF71-36B2A4DD30DE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{81C5968D-C541-47E2-91FE-57307286EF6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BE0D76-B6B6-4D2E-BBC3-3B7846A960AB}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E3ED3579-EC30-441B-964D-79C76377AF92}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{1362CB26-20B1-4B68-9928-FB351EF2B69B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F6FF86-A2C5-4227-BB6C-49EB77345971}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BE4E1DC7-F7A1-4AB3-A440-CB436CF37269}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C3F9EDA3-DE6F-4DF1-8235-E77FFFE50A6D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56099D5A-F252-4936-B614-950112542F91}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,7 +805,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -696,27 +813,27 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{C08AE416-F6B5-4D23-97C3-F7ADA7499914}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{66746C55-8258-4A44-A208-EA561290596A}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{16505763-057A-4353-8BDB-4364DED9BD42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDDA6A4-9A6F-458D-88E6-3E0F746190CC}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,13 +852,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -749,33 +866,33 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E2AC3705-FA45-4D0F-8671-674D14EC6F50}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{F41599FD-FE32-49AC-ACAC-2893DBF70D67}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C7811B98-27C2-4F12-8D84-D08368FC5C5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3769CF-BD81-48DE-A5D1-1D1B193E1D87}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,91 +914,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{158283EF-C717-434E-A3BD-33CB948EBC8D}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{A46E4B84-F401-4981-890C-F11C5E5B238B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D6CF58-AE02-44D1-BA3E-DF663D6454B7}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F3A27578-E331-4E10-AC84-4D499372F7B3}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{5792BBEE-B5A0-471C-83FA-2F947BE8C803}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329C3687-7E55-474B-A683-AFF9C67E6F53}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{32D473F2-4E07-4778-B54F-AA8A0560EE3D}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{C59ED131-2F5A-48AB-928A-19AD4F521A51}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{FE27194D-8F23-40C1-B79A-2DF969512806}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>